<commit_message>
changed the analyzing functions (kept the main dict as is), added tests for both heb and heb+eng results, changed the analyze_docs functions so there is no need to change it, added a column in the excel file and changed the GUI to the docs' name from the Front End, added documentation
</commit_message>
<xml_diff>
--- a/documents_data.xlsx
+++ b/documents_data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udi\PycharmWork\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD0E9CE3-D336-4BD0-BF3F-6E4BB81EADCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E348A88D-B6E8-4D02-AEA5-9CB4D89EC669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" xr2:uid="{FBE9C637-2F8D-4A56-B9F6-5AD6113F0A74}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBE9C637-2F8D-4A56-B9F6-5AD6113F0A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
   <si>
     <t>file name</t>
   </si>
@@ -97,6 +98,183 @@
   </si>
   <si>
     <t>input_images/itrot.png</t>
+  </si>
+  <si>
+    <t>file kind</t>
+  </si>
+  <si>
+    <t>candidate_id</t>
+  </si>
+  <si>
+    <t>father_id</t>
+  </si>
+  <si>
+    <t>mother_id</t>
+  </si>
+  <si>
+    <t>File Kind List</t>
+  </si>
+  <si>
+    <t>candidate_current_account</t>
+  </si>
+  <si>
+    <t>father_current_account</t>
+  </si>
+  <si>
+    <t>mother_current_account</t>
+  </si>
+  <si>
+    <t>partner_current_account</t>
+  </si>
+  <si>
+    <t>candidate_details_of_credit_charges</t>
+  </si>
+  <si>
+    <t>mother_details_of_credit_charges</t>
+  </si>
+  <si>
+    <t>partner_details_of_credit_charges</t>
+  </si>
+  <si>
+    <t>candidate_balance_concentration</t>
+  </si>
+  <si>
+    <t>father_balance_concentration</t>
+  </si>
+  <si>
+    <t>mother_balance_concentration</t>
+  </si>
+  <si>
+    <t>partner_balance_concentration</t>
+  </si>
+  <si>
+    <t>candidate_vehicle_licence</t>
+  </si>
+  <si>
+    <t>father_vehicle_licence</t>
+  </si>
+  <si>
+    <t>mother_vehicle_licence</t>
+  </si>
+  <si>
+    <t>father_rental_agreement</t>
+  </si>
+  <si>
+    <t>partner_vehicle_licence</t>
+  </si>
+  <si>
+    <t>candidate_rental_agreement</t>
+  </si>
+  <si>
+    <t>mother_rental_agreement</t>
+  </si>
+  <si>
+    <t>partner_rental_agreement</t>
+  </si>
+  <si>
+    <t>marriage_certificate</t>
+  </si>
+  <si>
+    <t>divorce_certificate</t>
+  </si>
+  <si>
+    <t>candidate_pay_stubs</t>
+  </si>
+  <si>
+    <t>father_pay_stubs</t>
+  </si>
+  <si>
+    <t>mother_pay_stubs</t>
+  </si>
+  <si>
+    <t>partner_pay_stubs</t>
+  </si>
+  <si>
+    <t>student_certificate</t>
+  </si>
+  <si>
+    <t>partner_death_certificate</t>
+  </si>
+  <si>
+    <t>father_death_certificate</t>
+  </si>
+  <si>
+    <t>mother_death_certificate</t>
+  </si>
+  <si>
+    <t>candidate_no_work</t>
+  </si>
+  <si>
+    <t>partner_no_work</t>
+  </si>
+  <si>
+    <t>father_no_work</t>
+  </si>
+  <si>
+    <t>mother_no_work</t>
+  </si>
+  <si>
+    <t>father_cpa_approval_on_income</t>
+  </si>
+  <si>
+    <t>mother_cpa_approval_on_income</t>
+  </si>
+  <si>
+    <t>partner_cpa_approval_on_income</t>
+  </si>
+  <si>
+    <t>exception_expenses</t>
+  </si>
+  <si>
+    <t>approve_allowance_amount</t>
+  </si>
+  <si>
+    <t>results_sheet</t>
+  </si>
+  <si>
+    <t>cv</t>
+  </si>
+  <si>
+    <t>warrior_certificate</t>
+  </si>
+  <si>
+    <t>discharge_certificate</t>
+  </si>
+  <si>
+    <t>monthly_budget_from_kibbutz</t>
+  </si>
+  <si>
+    <t>providing_assistance_from_kibbutz</t>
+  </si>
+  <si>
+    <t>candidate_mortgage</t>
+  </si>
+  <si>
+    <t>father_mortgage</t>
+  </si>
+  <si>
+    <t>mother_mortgage</t>
+  </si>
+  <si>
+    <t>partner_mortgage</t>
+  </si>
+  <si>
+    <t>tuition</t>
+  </si>
+  <si>
+    <t>candidate_mole_report</t>
+  </si>
+  <si>
+    <t>partner_mole_report</t>
+  </si>
+  <si>
+    <t>father_mole_report</t>
+  </si>
+  <si>
+    <t>mother_mole_report</t>
+  </si>
+  <si>
+    <t>father_details_of_credit_charges</t>
   </si>
 </sst>
 </file>
@@ -449,110 +627,445 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5402B2-DC25-419C-92EF-FC07BA57B32B}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
+    <col min="2" max="2" width="29.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.5546875" customWidth="1"/>
-    <col min="8" max="8" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>15</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>16</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
       <c r="B2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>20</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>13</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>10</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>10</v>
       </c>
-      <c r="M2">
+      <c r="N2">
         <v>0</v>
       </c>
-      <c r="O2">
+      <c r="P2">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B7E9801C-BDD2-4E7C-979C-8E2B2151BB79}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$58</xm:f>
+          </x14:formula1>
+          <xm:sqref>B1 B3:B1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C382787F-F478-4D71-BD4A-4D6C92020EC3}">
+          <x14:formula1>
+            <xm:f>Sheet2!$A$2:$A$58</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05A54689-E8A0-4004-8127-CBD251AAB422}">
+  <dimension ref="A1:A58"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A58" sqref="A2:A58"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="31.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the score for document recognition, fixed bugs in the GUI and in the excel graph results tool, updated the excel file
</commit_message>
<xml_diff>
--- a/documents_data.xlsx
+++ b/documents_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\udi\PycharmWork\Test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E348A88D-B6E8-4D02-AEA5-9CB4D89EC669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F08608E7-CF95-4F10-8CFC-F97DD209E119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FBE9C637-2F8D-4A56-B9F6-5AD6113F0A74}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12360" tabRatio="508" xr2:uid="{FBE9C637-2F8D-4A56-B9F6-5AD6113F0A74}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="94">
   <si>
     <t>file name</t>
   </si>
@@ -97,9 +97,6 @@
     <t>score 7</t>
   </si>
   <si>
-    <t>input_images/itrot.png</t>
-  </si>
-  <si>
     <t>file kind</t>
   </si>
   <si>
@@ -275,13 +272,58 @@
   </si>
   <si>
     <t>father_details_of_credit_charges</t>
+  </si>
+  <si>
+    <t>input_images/balance_concentration/balance_concentration1.png</t>
+  </si>
+  <si>
+    <t>input_images/balance_concentration/balance_concentration2.pdf</t>
+  </si>
+  <si>
+    <t>input_images/balance_concentration/balance_concentration3.jpeg</t>
+  </si>
+  <si>
+    <t>input_images/balance_concentration/balance_concentration4.jpeg</t>
+  </si>
+  <si>
+    <t>input_images/balance_concentration/balance_concentration5.pdf</t>
+  </si>
+  <si>
+    <t>input_images/bank_osh.pdf</t>
+  </si>
+  <si>
+    <t>444-2331</t>
+  </si>
+  <si>
+    <t>10.09.2021</t>
+  </si>
+  <si>
+    <t>תנועות בחשבון</t>
+  </si>
+  <si>
+    <t>בנק הפועלים</t>
+  </si>
+  <si>
+    <t>input_images/marriage.jpg</t>
+  </si>
+  <si>
+    <t>תעודת נישואין</t>
+  </si>
+  <si>
+    <t>input_images/credit_card.pdf</t>
+  </si>
+  <si>
+    <t>קבוצות ישראכרט</t>
+  </si>
+  <si>
+    <t>ישראל ישראלי</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -290,16 +332,41 @@
       <charset val="177"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="177"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -307,12 +374,42 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -627,15 +724,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC5402B2-DC25-419C-92EF-FC07BA57B32B}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="58.21875" customWidth="1"/>
     <col min="2" max="2" width="29.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.44140625" customWidth="1"/>
@@ -647,12 +744,12 @@
     <col min="14" max="14" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -697,51 +794,326 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C2" t="s">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" s="3">
+        <v>20</v>
+      </c>
+      <c r="E2" s="4">
+        <v>30066.16</v>
+      </c>
+      <c r="F2" s="3">
+        <v>20</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="H2" s="3">
+        <v>20</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="3">
+        <v>10</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="L2" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="3">
+        <v>20</v>
+      </c>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+    </row>
+    <row r="4" spans="1:16" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="3">
+        <v>20</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F4" s="3">
+        <v>20</v>
+      </c>
+      <c r="G4" s="3">
+        <v>138.46</v>
+      </c>
+      <c r="H4" s="3">
+        <v>20</v>
+      </c>
+      <c r="I4" s="5">
+        <v>44400</v>
+      </c>
+      <c r="J4" s="3">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5">
+        <v>44418</v>
+      </c>
+      <c r="L4" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="D5">
+        <v>20</v>
+      </c>
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="F5">
+        <v>20</v>
+      </c>
+      <c r="G5" t="s">
         <v>13</v>
       </c>
-      <c r="H2">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="H5">
+        <v>20</v>
+      </c>
+      <c r="I5" t="s">
         <v>14</v>
       </c>
-      <c r="J2">
+      <c r="J5">
         <v>10</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K5" t="s">
         <v>17</v>
       </c>
-      <c r="L2">
+      <c r="L5">
         <v>10</v>
       </c>
-      <c r="N2">
+      <c r="N5">
         <v>0</v>
       </c>
-      <c r="P2">
+      <c r="P5">
         <v>0</v>
       </c>
     </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>20</v>
+      </c>
+      <c r="E6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
+      </c>
+      <c r="I6" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6">
+        <v>10</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6">
+        <v>10</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7">
+        <v>20</v>
+      </c>
+      <c r="E7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7" t="s">
+        <v>17</v>
+      </c>
+      <c r="L7">
+        <v>10</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>20</v>
+      </c>
+      <c r="I8" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8">
+        <v>10</v>
+      </c>
+      <c r="K8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8">
+        <v>10</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9">
+        <v>10</v>
+      </c>
+      <c r="K9" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9">
+        <v>10</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
   <extLst>
@@ -751,13 +1123,13 @@
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$58</xm:f>
           </x14:formula1>
-          <xm:sqref>B1 B3:B1048576</xm:sqref>
+          <xm:sqref>B1 B10:B1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C382787F-F478-4D71-BD4A-4D6C92020EC3}">
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$58</xm:f>
           </x14:formula1>
-          <xm:sqref>B2</xm:sqref>
+          <xm:sqref>B5:B9</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -780,292 +1152,292 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>